<commit_message>
additional solution in task_1
</commit_message>
<xml_diff>
--- a/Statistic/Task_1/Solution_1.xlsx
+++ b/Statistic/Task_1/Solution_1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VikhlyantsevAA\Desktop\Portfolio_Analitics\Statistic\Task_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE7DFF0-BDC7-4474-B942-DF9212341C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2803389A-2A8E-41C6-9E73-FBAD48B42599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Решение" sheetId="2" r:id="rId1"/>
+    <sheet name="Решение" sheetId="4" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -41,7 +41,7 @@
     <author>Технолог</author>
   </authors>
   <commentList>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{0C14A3B0-8EEF-477E-9DA8-062E66762009}">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{80E69651-D3AE-48C3-BE0D-75321272B110}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{356DE48A-047E-41EB-9285-63EE93B64E19}">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{42F87A46-7379-48E7-A964-275C83FCF1A5}">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
   <si>
     <t>Таможенный пост</t>
   </si>
@@ -156,13 +156,339 @@
   </si>
   <si>
     <t>96,6 - 111,16</t>
+  </si>
+  <si>
+    <t>Данные получены с помощью</t>
+  </si>
+  <si>
+    <t>пакета "Анализ данных":</t>
+  </si>
+  <si>
+    <t>Накопленные частоты</t>
+  </si>
+  <si>
+    <t>Описательные статистики:</t>
+  </si>
+  <si>
+    <t>Показатели положения:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Средняя арифметическая = </t>
+  </si>
+  <si>
+    <t>=СРЗНАЧ($B$3:$B$37)</t>
+  </si>
+  <si>
+    <t>2. Медиана =</t>
+  </si>
+  <si>
+    <t>=МЕДИАНА($B$3:$B$37)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Мода = </t>
+  </si>
+  <si>
+    <r>
+      <t>4. Нижний квартиль Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+  </si>
+  <si>
+    <t>=КВАРТИЛЬ.ВКЛ($B$3:$B$37;1)</t>
+  </si>
+  <si>
+    <r>
+      <t>5. Средний квартил Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <t>=КВАРТИЛЬ.ВКЛ($B$3:$B$37;2)</t>
+  </si>
+  <si>
+    <r>
+      <t>6. Верхний квартиль Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <t>=КВАРТИЛЬ.ВКЛ($B$3:$B$37;3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Процентиль (1/3) = </t>
+  </si>
+  <si>
+    <t>=ПРОЦЕНТИЛЬ.ВКЛ($B$3:$B$37;1/3)</t>
+  </si>
+  <si>
+    <t>Показатели разброса данных:</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Дисперсия выборки S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>=ДИСП.В($B$3:$B$37)</t>
+  </si>
+  <si>
+    <t>2. Стандартное отклонение</t>
+  </si>
+  <si>
+    <t>=СТАНДОТКЛОН.В($B$3:$B$37)</t>
+  </si>
+  <si>
+    <t>3. Размах</t>
+  </si>
+  <si>
+    <t>=МАКС($B$3:$B$37)-МИН($B$3:$B$37)</t>
+  </si>
+  <si>
+    <t>Описательные статистики можно вывести с помощью надстройки "Анализ данных":</t>
+  </si>
+  <si>
+    <t>Столбец1</t>
+  </si>
+  <si>
+    <t>Среднее</t>
+  </si>
+  <si>
+    <t>Стандартная ошибка</t>
+  </si>
+  <si>
+    <t>Медиана</t>
+  </si>
+  <si>
+    <t>Мода</t>
+  </si>
+  <si>
+    <t>Стандартное отклонение</t>
+  </si>
+  <si>
+    <t>Дисперсия выборки</t>
+  </si>
+  <si>
+    <t>Эксцесс</t>
+  </si>
+  <si>
+    <t>Асимметричность</t>
+  </si>
+  <si>
+    <t>Интервал</t>
+  </si>
+  <si>
+    <t>Минимум</t>
+  </si>
+  <si>
+    <t>Максимум</t>
+  </si>
+  <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>Счет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Модой наших значений будет интервал от 53,16 до 67,66 так как </t>
+  </si>
+  <si>
+    <t>именно этот интервал с наиболее высокой частотой наблюдения</t>
+  </si>
+  <si>
+    <t>Моду данного интервала можно рассчитать по формуле:</t>
+  </si>
+  <si>
+    <t>Xmin =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">минимальное значение интервала </t>
+  </si>
+  <si>
+    <t>d =</t>
+  </si>
+  <si>
+    <t>ширина медианного интервала Xmax - Xmin</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <t>частота модального диапазона</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mo-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <t>частота предмодального диапазона</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mo + 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+  </si>
+  <si>
+    <t>частота постмодального диапазона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мода нашего модального диапазона </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,28 +509,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,6 +525,67 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -290,56 +661,109 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="2" xr:uid="{9A15D432-6739-48A5-9062-F21C6E795E12}"/>
+    <cellStyle name="Обычный 2 2" xfId="3" xr:uid="{7C21ECDC-CB63-4B3D-BA14-EF07D7ECCEC2}"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -500,7 +924,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Решение!$K$20:$K$25</c:f>
+              <c:f>Решение!$L$20:$L$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -526,7 +950,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Решение!$L$20:$L$25</c:f>
+              <c:f>Решение!$M$20:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -553,7 +977,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7ECC-4E92-A1FC-215282AEFA15}"/>
+              <c16:uniqueId val="{00000000-175F-4942-A219-FD2981C735B0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -657,7 +1081,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Решение!$K$20:$K$25</c:f>
+              <c:f>Решение!$L$20:$L$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -683,7 +1107,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Решение!$M$20:$M$25</c:f>
+              <c:f>Решение!$N$20:$N$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -711,7 +1135,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7ECC-4E92-A1FC-215282AEFA15}"/>
+              <c16:uniqueId val="{00000001-175F-4942-A219-FD2981C735B0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1233,7 +1657,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Решение!$K$20:$K$25</c:f>
+              <c:f>Решение!$L$20:$L$25</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1259,7 +1683,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Решение!$L$20:$L$25</c:f>
+              <c:f>Решение!$M$20:$M$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1287,7 +1711,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3887-4658-9464-535683AF01BE}"/>
+              <c16:uniqueId val="{00000000-0F55-4BC9-A9D7-F685075441B3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2744,25 +3168,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>498663</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0585EF3-6A49-4CB3-9493-F4C8D5258EB6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE53851-3E29-4762-A3CD-BDE8C5D5146F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2782,25 +3206,25 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>7844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AD69BC7-37CA-4A41-AD3A-5CBE31C55DA2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C333DD-7931-451B-A437-4B7B08B7D7FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2818,6 +3242,766 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>96370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1252443</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>62751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Рисунок 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA225F1-DC7B-4346-A09F-9C94D34B42E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2567268" y="14469595"/>
+          <a:ext cx="4866900" cy="566456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12887</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5EC01A1-642D-49CD-B5BE-EEBEFA96ABA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2546537" y="17297401"/>
+          <a:ext cx="6140262" cy="5610224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Вывод:</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Наибольшее количество таможенных</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> постов имеет внешнеторговый оборот в диапазоне от 53,16 до 67,66 млн. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>$</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Оценивая значения средней арифметической и медианы, мы можем прийти к выводу,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>что данные у нас однородны (нет выбросов, экстремумов) так как разница </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>средних незначительна (не более 5,6%)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Так как Мода ≈ Медиана  ≈ Среднее арифметическое, то можем сделать предварительный вывод о том, что </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>мы имеем дело со стабильно меняющейся совокупностью и данные подчиняются нормальному закону распределения (с небольшой погрешностью).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Благодаря мерам относительного положения (квартили, процентиль) мы можем сделать следующие выводы:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. 25% таможенных постов</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> с</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> внешнеторговым оборотом, менее 47,585 млн. $</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. 50% </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>таможенных постов</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> с</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> внешнеторговым оборотом, менее </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>56,8 млн. $</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3. 75% </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>таможенных постов</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> с</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> внешнеторговым оборотом, менее </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>70,315 млн. $</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4. 33,33% </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>таможенных постов</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> с</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> внешнеторговым оборотом, менее </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>53,08 млн. $</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Предполагая, что наши данные подчиняются нормальному закону распределения</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>мы можем использовать эмпирическое правило (правило трех сигм):</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Me ± S </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t>      68,26%</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Me ± 2 S</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t>    95,44%</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Me ± 3 S </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t>   99,72%</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. 68,26 % </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>наших значений будет находиться в диапазоне от 35,38 до 78,22 млн.$</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. 95,44 % наших значений будет находиться в диапазоне от 13,96 до 99,64 млн.$</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3. 99,72 % наших значений будет находиться в диапазоне от -7,47 до 121,07 млн.$</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2886,73 +4070,81 @@
       <sheetName val="Решение_29"/>
       <sheetName val="Задание_30"/>
       <sheetName val="Решение_30"/>
+      <sheetName val="Задание_31"/>
+      <sheetName val="Решение_31"/>
+      <sheetName val="Задание_32"/>
+      <sheetName val="Решение_32"/>
+      <sheetName val="Задание_33"/>
+      <sheetName val="Решение_33"/>
+      <sheetName val="Задание_34"/>
+      <sheetName val="Решение_34"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="20">
-          <cell r="K20" t="str">
+          <cell r="L20" t="str">
             <v>24,16 -38,66</v>
           </cell>
-          <cell r="L20">
+          <cell r="M20">
             <v>5</v>
           </cell>
-          <cell r="M20">
+          <cell r="N20">
             <v>0.14285714285714285</v>
           </cell>
         </row>
         <row r="21">
-          <cell r="K21" t="str">
+          <cell r="L21" t="str">
             <v>38,66 - 53,16</v>
           </cell>
-          <cell r="L21">
+          <cell r="M21">
             <v>7</v>
           </cell>
-          <cell r="M21">
+          <cell r="N21">
             <v>0.34285714285714286</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="K22" t="str">
+          <cell r="L22" t="str">
             <v>53,16 - 67,66</v>
           </cell>
-          <cell r="L22">
+          <cell r="M22">
             <v>13</v>
           </cell>
-          <cell r="M22">
+          <cell r="N22">
             <v>0.7142857142857143</v>
           </cell>
         </row>
         <row r="23">
-          <cell r="K23" t="str">
+          <cell r="L23" t="str">
             <v>67,66 - 82,16</v>
           </cell>
-          <cell r="L23">
+          <cell r="M23">
             <v>4</v>
           </cell>
-          <cell r="M23">
+          <cell r="N23">
             <v>0.82857142857142863</v>
           </cell>
         </row>
         <row r="24">
-          <cell r="K24" t="str">
+          <cell r="L24" t="str">
             <v>82,16 - 96,66</v>
           </cell>
-          <cell r="L24">
+          <cell r="M24">
             <v>4</v>
           </cell>
-          <cell r="M24">
+          <cell r="N24">
             <v>0.94285714285714284</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="K25" t="str">
+          <cell r="L25" t="str">
             <v>96,6 - 111,16</v>
           </cell>
-          <cell r="L25">
+          <cell r="M25">
             <v>2</v>
           </cell>
-          <cell r="M25">
+          <cell r="N25">
             <v>1</v>
           </cell>
         </row>
@@ -3014,6 +4206,14 @@
       <sheetData sheetId="56"/>
       <sheetData sheetId="57"/>
       <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3281,589 +4481,1041 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1B18E2-2AF1-4F5F-A3D6-E26C7E84AE19}">
-  <dimension ref="A2:M37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E6BF6D-F500-41B4-8E05-C04D0F795881}">
+  <dimension ref="A2:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="7" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="1"/>
+    <col min="17" max="21" width="9.140625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="9.140625" style="1"/>
+    <col min="24" max="24" width="9.140625" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>24.16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>27.06</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>29.12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f>COUNT(A3:A37)</f>
         <v>35</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>31.17</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f>ROUNDDOWN(1+(3.322*LOG(35)),0)</f>
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>37.08</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>39.11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>41.58</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>44.84</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>46.8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>48.37</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f>MAX(B3:B37)</f>
         <v>111.16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="5">
         <v>51.44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f>MIN(B3:B37)</f>
         <v>24.16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>52.56</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <f>(E12-E13)/E6</f>
         <v>14.5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>54.12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>54.91</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="5">
         <v>55.74</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="L17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+    </row>
+    <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>55.91</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="L18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="5">
         <v>56.07</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="J19" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="M19" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="N19" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="5">
         <v>56.8</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="16">
         <v>1</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f>MIN(B3:B37)</f>
         <v>24.16</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <f>E20+$E$14</f>
         <v>38.659999999999997</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E20,$B$3:$B$37,"&lt;"&amp;F20)</f>
         <v>5</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1">
         <f t="array" ref="H20:H25">FREQUENCY(B3:B37,F20:F25)</f>
         <v>5</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="17">
         <f>H20/$E$5</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="J20" s="18">
+        <f>H20</f>
+        <v>5</v>
+      </c>
+      <c r="L20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L20">
+      <c r="M20" s="1">
         <v>5</v>
       </c>
-      <c r="M20" s="14">
+      <c r="N20" s="19">
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="5">
         <v>56.93</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="16">
         <v>2</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f>F20</f>
         <v>38.659999999999997</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <f>E21+$E$14</f>
         <v>53.16</v>
       </c>
-      <c r="G21">
-        <f t="shared" ref="G21:G24" si="0">COUNTIFS($B$3:$B$37,"&gt;="&amp;E21,$B$3:$B$37,"&lt;"&amp;F21)</f>
+      <c r="G21" s="1">
+        <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E21,$B$3:$B$37,"&lt;"&amp;F21)</f>
         <v>7</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1">
         <v>7</v>
       </c>
-      <c r="I21" s="13">
-        <f t="shared" ref="I21:I25" si="1">H21/$E$5</f>
+      <c r="I21" s="17">
+        <f t="shared" ref="I21:I25" si="0">H21/$E$5</f>
         <v>0.2</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="J21" s="18">
+        <f>J20+H21</f>
+        <v>12</v>
+      </c>
+      <c r="L21" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L21">
+      <c r="M21" s="1">
         <v>7</v>
       </c>
-      <c r="M21" s="14">
+      <c r="N21" s="19">
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="5">
         <v>57.07</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="16">
         <v>3</v>
       </c>
-      <c r="E22">
-        <f t="shared" ref="E22:E25" si="2">F21</f>
+      <c r="E22" s="1">
+        <f t="shared" ref="E22:E25" si="1">F21</f>
         <v>53.16</v>
       </c>
-      <c r="F22">
-        <f t="shared" ref="F22:F25" si="3">E22+$E$14</f>
+      <c r="F22" s="1">
+        <f t="shared" ref="F22:F25" si="2">E22+$E$14</f>
         <v>67.66</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
+        <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E22,$B$3:$B$37,"&lt;"&amp;F22)</f>
+        <v>13</v>
+      </c>
+      <c r="H22" s="1">
+        <v>13</v>
+      </c>
+      <c r="I22" s="17">
         <f t="shared" si="0"/>
+        <v>0.37142857142857144</v>
+      </c>
+      <c r="J22" s="18">
+        <f t="shared" ref="J22:J25" si="3">J21+H22</f>
+        <v>25</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="1">
         <v>13</v>
       </c>
-      <c r="H22">
-        <v>13</v>
-      </c>
-      <c r="I22" s="13">
+      <c r="N22" s="19">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5">
+        <v>58.39</v>
+      </c>
+      <c r="D23" s="16">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
         <f t="shared" si="1"/>
-        <v>0.37142857142857144</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L22">
-        <v>13</v>
-      </c>
-      <c r="M22" s="14">
-        <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>21</v>
-      </c>
-      <c r="B23" s="4">
-        <v>58.39</v>
-      </c>
-      <c r="D23" s="12">
-        <v>4</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="2"/>
         <v>67.66</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>82.16</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H23">
-        <v>4</v>
-      </c>
-      <c r="I23" s="13">
-        <f t="shared" si="1"/>
-        <v>0.11428571428571428</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L23">
-        <v>4</v>
-      </c>
-      <c r="M23" s="14">
-        <v>0.82857142857142863</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>22</v>
-      </c>
-      <c r="B24" s="4">
-        <v>59.61</v>
-      </c>
-      <c r="D24" s="12">
-        <v>5</v>
-      </c>
-      <c r="E24">
+      <c r="F23" s="1">
         <f t="shared" si="2"/>
         <v>82.16</v>
       </c>
-      <c r="F24">
+      <c r="G23" s="1">
+        <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E23,$B$3:$B$37,"&lt;"&amp;F23)</f>
+        <v>4</v>
+      </c>
+      <c r="H23" s="1">
+        <v>4</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="0"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="J23" s="18">
         <f t="shared" si="3"/>
-        <v>96.66</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" s="1">
         <v>4</v>
       </c>
-      <c r="H24">
-        <v>4</v>
-      </c>
-      <c r="I24" s="13">
+      <c r="N23" s="19">
+        <v>0.82857142857142863</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5">
+        <v>59.61</v>
+      </c>
+      <c r="D24" s="16">
+        <v>5</v>
+      </c>
+      <c r="E24" s="1">
         <f t="shared" si="1"/>
-        <v>0.11428571428571428</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24">
-        <v>4</v>
-      </c>
-      <c r="M24" s="14">
-        <v>0.94285714285714284</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4">
-        <v>59.95</v>
-      </c>
-      <c r="D25" s="15">
-        <v>6</v>
-      </c>
-      <c r="E25" s="8">
+        <v>82.16</v>
+      </c>
+      <c r="F24" s="1">
         <f t="shared" si="2"/>
         <v>96.66</v>
       </c>
-      <c r="F25" s="8">
+      <c r="G24" s="1">
+        <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E24,$B$3:$B$37,"&lt;"&amp;F24)</f>
+        <v>4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>4</v>
+      </c>
+      <c r="I24" s="17">
+        <f t="shared" si="0"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="J24" s="18">
         <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="1">
+        <v>4</v>
+      </c>
+      <c r="N24" s="19">
+        <v>0.94285714285714284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5">
+        <v>59.95</v>
+      </c>
+      <c r="D25" s="20">
+        <v>6</v>
+      </c>
+      <c r="E25" s="11">
+        <f t="shared" si="1"/>
+        <v>96.66</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="2"/>
         <v>111.16</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="11">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E25,$B$3:$B$37,"&lt;="&amp;F25)</f>
         <v>2</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="11">
         <v>2</v>
       </c>
-      <c r="I25" s="16">
-        <f t="shared" si="1"/>
+      <c r="I25" s="21">
+        <f t="shared" si="0"/>
         <v>5.7142857142857141E-2</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="J25" s="22">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="L25" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="8">
+      <c r="M25" s="11">
         <v>2</v>
       </c>
-      <c r="M25" s="17">
+      <c r="N25" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="5">
         <v>62.05</v>
       </c>
-      <c r="H26" s="18"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="5">
         <v>65.31</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="5">
         <v>69.239999999999995</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="D28" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>27</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="5">
         <v>71.39</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>28</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="5">
         <v>77.12</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="D30" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>29</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="5">
         <v>79.12</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="D31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="1">
+        <f>AVERAGE(B3:B37)</f>
+        <v>60</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="5">
         <v>84.34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="D32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="7">
+        <f>MEDIAN($B$3:$B$37)</f>
+        <v>56.8</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="5">
         <v>86.89</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="1">
+        <f>E79</f>
+        <v>58.959999999999994</v>
+      </c>
+      <c r="I33" s="27"/>
+    </row>
+    <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="5">
         <v>91.74</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="1">
+        <f>_xlfn.QUARTILE.INC($B$3:$B$37,1)</f>
+        <v>47.584999999999994</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="5">
         <v>96.01</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="D35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="1">
+        <f>_xlfn.QUARTILE.INC($B$3:$B$37,2)</f>
+        <v>56.8</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="5">
         <v>106.84</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="D36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G36" s="1">
+        <f>_xlfn.QUARTILE.INC($B$3:$B$37,3)</f>
+        <v>70.314999999999998</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="5">
         <v>111.16</v>
       </c>
+      <c r="D37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="1">
+        <f>_xlfn.PERCENTILE.INC($B$3:$B$37,1/3)</f>
+        <v>53.08</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" s="29">
+        <f>_xlfn.VAR.S($B$3:$B$37)</f>
+        <v>458.88883529411737</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="29">
+        <f>_xlfn.STDEV.S(B3:B37)</f>
+        <v>21.421690766466529</v>
+      </c>
+      <c r="I41" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="30">
+        <f>MAX($B$3:$B$37)-MIN(B3:B37)</f>
+        <v>87</v>
+      </c>
+      <c r="I42" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D43" s="4"/>
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D44" s="4"/>
+      <c r="I44" s="31"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I45" s="31"/>
+    </row>
+    <row r="46" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="32"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="I46" s="31"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D47" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="33"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="1">
+        <v>60</v>
+      </c>
+      <c r="I49" s="31"/>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G50" s="1">
+        <v>3.620926618951553</v>
+      </c>
+      <c r="I50" s="31"/>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G51" s="1">
+        <v>56.8</v>
+      </c>
+      <c r="I51" s="31"/>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G52" s="1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I52" s="31"/>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="1">
+        <v>21.421690766466529</v>
+      </c>
+      <c r="I53" s="31"/>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G54" s="1">
+        <v>458.88883529411737</v>
+      </c>
+      <c r="I54" s="31"/>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0.14905801050987311</v>
+      </c>
+      <c r="I55" s="31"/>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0.60932074068833608</v>
+      </c>
+      <c r="I56" s="31"/>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" s="1">
+        <v>87</v>
+      </c>
+      <c r="I57" s="31"/>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G58" s="1">
+        <v>24.16</v>
+      </c>
+      <c r="I58" s="31"/>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G59" s="1">
+        <v>111.16</v>
+      </c>
+      <c r="I59" s="31"/>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G60" s="1">
+        <v>2100</v>
+      </c>
+      <c r="I60" s="31"/>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D61" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26">
+        <v>35</v>
+      </c>
+      <c r="I61" s="31"/>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="4"/>
+      <c r="I62" s="31"/>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I63" s="31"/>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D64" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I64" s="31"/>
+    </row>
+    <row r="65" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D68" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D74" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E74" s="16">
+        <f>E22</f>
+        <v>53.16</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D75" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E75" s="16">
+        <f>F22-E22</f>
+        <v>14.5</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="4:10" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="D76" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E76" s="16">
+        <f>G22</f>
+        <v>13</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="4:10" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="D77" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="16">
+        <f>G21</f>
+        <v>7</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="4:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D78" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="E78" s="20">
+        <f>G23</f>
+        <v>4</v>
+      </c>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+    </row>
+    <row r="79" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D79" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" s="38">
+        <f>E74+E75*((E76-E77)/((E76-E77)+(E76-E78)))</f>
+        <v>58.959999999999994</v>
+      </c>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H79" s="39"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="4"/>
+    </row>
+    <row r="100" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="Q100" s="29"/>
+      <c r="R100" s="29"/>
+      <c r="S100" s="29"/>
+    </row>
+    <row r="105" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E105" s="19"/>
+    </row>
+    <row r="106" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E106" s="19"/>
+    </row>
+    <row r="107" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E107" s="19"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B3:B38">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
add new files task_1 - task_4
</commit_message>
<xml_diff>
--- a/Statistic/Task_1/Solution_1.xlsx
+++ b/Statistic/Task_1/Solution_1.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VikhlyantsevAA\Desktop\Portfolio_Analitics\Statistic\Task_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Portfolio_Analitics\Statistic\Task_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2803389A-2A8E-41C6-9E73-FBAD48B42599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649BBDBA-28C4-419A-BEF8-31378EBA6FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Решение" sheetId="4" r:id="rId1"/>
+    <sheet name="Решение" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +39,7 @@
     <author>Технолог</author>
   </authors>
   <commentList>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{80E69651-D3AE-48C3-BE0D-75321272B110}">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{26FAE9C0-CBEA-40D4-8F11-4838F54E5748}">
       <text>
         <r>
           <rPr>
@@ -55,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{42F87A46-7379-48E7-A964-275C83FCF1A5}">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{6BAED848-9F4F-42A0-AD60-6A3E02C6A062}">
       <text>
         <r>
           <rPr>
@@ -86,7 +84,7 @@
     <t>1. Определяем количество групп, используя одну из формул Стёрджеса</t>
   </si>
   <si>
-    <t>k = 1 + (3,322 * logN) или k = 1 + (1,44 * lnN)</t>
+    <t>k = 1 + 3,322 * logN или k = 1 + 1,44 * lnN</t>
   </si>
   <si>
     <t>N =</t>
@@ -116,6 +114,12 @@
     <t xml:space="preserve">3. Пасторим диапазоны </t>
   </si>
   <si>
+    <t>Данные получены с помощью</t>
+  </si>
+  <si>
+    <t>пакета "Анализ данных":</t>
+  </si>
+  <si>
     <t>k</t>
   </si>
   <si>
@@ -131,6 +135,9 @@
     <t>Распределение выборочных частот</t>
   </si>
   <si>
+    <t>Накопленные частоты</t>
+  </si>
+  <si>
     <t>Карман</t>
   </si>
   <si>
@@ -156,15 +163,6 @@
   </si>
   <si>
     <t>96,6 - 111,16</t>
-  </si>
-  <si>
-    <t>Данные получены с помощью</t>
-  </si>
-  <si>
-    <t>пакета "Анализ данных":</t>
-  </si>
-  <si>
-    <t>Накопленные частоты</t>
   </si>
   <si>
     <t>Описательные статистики:</t>
@@ -488,7 +486,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,24 +507,10 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -534,7 +518,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -586,6 +569,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -661,95 +651,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="2" xr:uid="{9A15D432-6739-48A5-9062-F21C6E795E12}"/>
-    <cellStyle name="Обычный 2 2" xfId="3" xr:uid="{7C21ECDC-CB63-4B3D-BA14-EF07D7ECCEC2}"/>
+    <cellStyle name="Обычный 2" xfId="2" xr:uid="{888C932A-97E8-4B6A-9E13-5E8A05A45791}"/>
     <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -977,7 +962,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-175F-4942-A219-FD2981C735B0}"/>
+              <c16:uniqueId val="{00000000-AED2-49B0-A7F7-6B2558A32075}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1135,7 +1120,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-175F-4942-A219-FD2981C735B0}"/>
+              <c16:uniqueId val="{00000001-AED2-49B0-A7F7-6B2558A32075}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1711,7 +1696,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0F55-4BC9-A9D7-F685075441B3}"/>
+              <c16:uniqueId val="{00000000-C750-4ABC-96CC-ECED9BBAEB62}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3171,22 +3156,22 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>498663</xdr:colOff>
+      <xdr:colOff>581791</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1681</xdr:rowOff>
+      <xdr:rowOff>57099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:colOff>616528</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Диаграмма 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE53851-3E29-4762-A3CD-BDE8C5D5146F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D6C562E-F371-4B13-A012-F61B616D4B56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3217,14 +3202,14 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
+      <xdr:rowOff>27709</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Диаграмма 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C333DD-7931-451B-A437-4B7B08B7D7FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8723807-5390-4FEE-9FFE-BEB18AE1A6EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3262,7 +3247,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA225F1-DC7B-4346-A09F-9C94D34B42E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E653866-8179-46C0-B33B-00CAB3501D09}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3285,8 +3270,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2567268" y="14469595"/>
-          <a:ext cx="4866900" cy="566456"/>
+          <a:off x="2639658" y="14300050"/>
+          <a:ext cx="4967865" cy="560741"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3315,15 +3300,15 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>41563</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5EC01A1-642D-49CD-B5BE-EEBEFA96ABA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DCE0999-A0F4-4E75-AEDC-78DC64FDCD1F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3331,8 +3316,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2546537" y="17297401"/>
-          <a:ext cx="6140262" cy="5610224"/>
+          <a:off x="2618927" y="17076421"/>
+          <a:ext cx="6309807" cy="6579522"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3544,8 +3529,53 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>мы имеем дело со стабильно меняющейся совокупностью и данные подчиняются нормальному закону распределения (с небольшой погрешностью).</a:t>
-          </a:r>
+            <a:t>мы имеем дело со стабильно меняющейся совокупностью и данные подчиняются нормальному закону распределения (с небольшой погрешностью). Дополнительно, мы получили данные Асимметричности</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> = 0,609</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> и Эксцесса</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> = 0,149. Считается, что если значения Асимметричности и Эксцесса находятся в границах от -1 до +1, то это косвенный показатель того, что данные близки к нормальному распределению</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="0" u="none" strike="noStrike">
@@ -4004,219 +4034,55 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>960120</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E2C583E-41C5-4D9C-8BF9-F0B1AC840214}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2606040" y="14295120"/>
+          <a:ext cx="4709160" cy="563880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Задача_1"/>
-      <sheetName val="Решение_1"/>
-      <sheetName val="Задача_2"/>
-      <sheetName val="Решение_2"/>
-      <sheetName val="Задача_3"/>
-      <sheetName val="Решение_3"/>
-      <sheetName val="Задача_4"/>
-      <sheetName val="Решение_4"/>
-      <sheetName val="Задача_5"/>
-      <sheetName val="Решение_5"/>
-      <sheetName val="Задача_6"/>
-      <sheetName val="Решение_6"/>
-      <sheetName val="Задача_7"/>
-      <sheetName val="Решение_7"/>
-      <sheetName val="Задача_8"/>
-      <sheetName val="Решение_8"/>
-      <sheetName val="Задача_9"/>
-      <sheetName val="Решение_9"/>
-      <sheetName val="Задача_10"/>
-      <sheetName val="Решение_10"/>
-      <sheetName val="Задача_11"/>
-      <sheetName val="Решение_11"/>
-      <sheetName val="Задача_12"/>
-      <sheetName val="Решение_12"/>
-      <sheetName val="Задача_13"/>
-      <sheetName val="Решение_13"/>
-      <sheetName val="Задача_14"/>
-      <sheetName val="Решение_14"/>
-      <sheetName val="Задача_15"/>
-      <sheetName val="Решение_15"/>
-      <sheetName val="Задача_16"/>
-      <sheetName val="Решение_16"/>
-      <sheetName val="Задание_17"/>
-      <sheetName val="Решение_17"/>
-      <sheetName val="Задание_18"/>
-      <sheetName val="Решение_18"/>
-      <sheetName val="Задание_19"/>
-      <sheetName val="Решение_19"/>
-      <sheetName val="Задание_20"/>
-      <sheetName val="Решение_20"/>
-      <sheetName val="Задание_21"/>
-      <sheetName val="Решение_21"/>
-      <sheetName val="Задание_22"/>
-      <sheetName val="Решение_22"/>
-      <sheetName val="Задание_23"/>
-      <sheetName val="Решение_23"/>
-      <sheetName val="Задание_24"/>
-      <sheetName val="Решение_24"/>
-      <sheetName val="Задание_25"/>
-      <sheetName val="Решение_25"/>
-      <sheetName val="Задание_26"/>
-      <sheetName val="Решение_26"/>
-      <sheetName val="Задание_27"/>
-      <sheetName val="Задание_28"/>
-      <sheetName val="Решение_28"/>
-      <sheetName val="Задание_29"/>
-      <sheetName val="Решение_29"/>
-      <sheetName val="Задание_30"/>
-      <sheetName val="Решение_30"/>
-      <sheetName val="Задание_31"/>
-      <sheetName val="Решение_31"/>
-      <sheetName val="Задание_32"/>
-      <sheetName val="Решение_32"/>
-      <sheetName val="Задание_33"/>
-      <sheetName val="Решение_33"/>
-      <sheetName val="Задание_34"/>
-      <sheetName val="Решение_34"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="20">
-          <cell r="L20" t="str">
-            <v>24,16 -38,66</v>
-          </cell>
-          <cell r="M20">
-            <v>5</v>
-          </cell>
-          <cell r="N20">
-            <v>0.14285714285714285</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="L21" t="str">
-            <v>38,66 - 53,16</v>
-          </cell>
-          <cell r="M21">
-            <v>7</v>
-          </cell>
-          <cell r="N21">
-            <v>0.34285714285714286</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="L22" t="str">
-            <v>53,16 - 67,66</v>
-          </cell>
-          <cell r="M22">
-            <v>13</v>
-          </cell>
-          <cell r="N22">
-            <v>0.7142857142857143</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="L23" t="str">
-            <v>67,66 - 82,16</v>
-          </cell>
-          <cell r="M23">
-            <v>4</v>
-          </cell>
-          <cell r="N23">
-            <v>0.82857142857142863</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="L24" t="str">
-            <v>82,16 - 96,66</v>
-          </cell>
-          <cell r="M24">
-            <v>4</v>
-          </cell>
-          <cell r="N24">
-            <v>0.94285714285714284</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="L25" t="str">
-            <v>96,6 - 111,16</v>
-          </cell>
-          <cell r="M25">
-            <v>2</v>
-          </cell>
-          <cell r="N25">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4265,7 +4131,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -4300,7 +4166,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -4481,47 +4347,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E6BF6D-F500-41B4-8E05-C04D0F795881}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1234F4-F0C0-4092-8ED3-3B58682F6F58}">
   <dimension ref="A2:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q96" sqref="Q96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16" width="9.140625" style="1"/>
-    <col min="17" max="21" width="9.140625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="9.140625" style="1"/>
-    <col min="24" max="24" width="9.140625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="3"/>
+    <col min="4" max="4" width="11.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="3"/>
+    <col min="6" max="6" width="10.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" style="3" customWidth="1"/>
+    <col min="15" max="16" width="9.109375" style="3"/>
+    <col min="17" max="21" width="9.109375" style="3" customWidth="1"/>
+    <col min="22" max="23" width="9.109375" style="3"/>
+    <col min="24" max="24" width="9.109375" style="3" customWidth="1"/>
+    <col min="25" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4532,7 +4399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4540,7 +4407,7 @@
         <v>27.06</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -4550,7 +4417,7 @@
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <f>COUNT(A3:A37)</f>
         <v>35</v>
       </c>
@@ -4558,7 +4425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -4568,12 +4435,12 @@
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <f>ROUNDDOWN(1+(3.322*LOG(35)),0)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -4581,7 +4448,7 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -4589,7 +4456,7 @@
         <v>39.11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -4600,7 +4467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -4611,7 +4478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -4619,7 +4486,7 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -4629,12 +4496,12 @@
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <f>MAX(B3:B37)</f>
         <v>111.16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -4644,12 +4511,12 @@
       <c r="D13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <f>MIN(B3:B37)</f>
         <v>24.16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -4659,12 +4526,12 @@
       <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <f>(E12-E13)/E6</f>
         <v>14.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -4672,7 +4539,7 @@
         <v>54.12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -4680,7 +4547,7 @@
         <v>54.91</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -4691,12 +4558,12 @@
         <v>12</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -4710,12 +4577,12 @@
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="L18" s="9" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -4723,37 +4590,37 @@
         <v>56.07</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M19" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="N19" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -4763,19 +4630,19 @@
       <c r="D20" s="16">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <f>MIN(B3:B37)</f>
         <v>24.16</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <f>E20+$E$14</f>
         <v>38.659999999999997</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="3">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E20,$B$3:$B$37,"&lt;"&amp;F20)</f>
         <v>5</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="3">
         <f t="array" ref="H20:H25">FREQUENCY(B3:B37,F20:F25)</f>
         <v>5</v>
       </c>
@@ -4788,16 +4655,16 @@
         <v>5</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="1">
+        <v>24</v>
+      </c>
+      <c r="M20" s="3">
         <v>5</v>
       </c>
       <c r="N20" s="19">
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -4807,19 +4674,19 @@
       <c r="D21" s="16">
         <v>2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <f>F20</f>
         <v>38.659999999999997</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <f>E21+$E$14</f>
         <v>53.16</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="3">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E21,$B$3:$B$37,"&lt;"&amp;F21)</f>
         <v>7</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="3">
         <v>7</v>
       </c>
       <c r="I21" s="17">
@@ -4831,16 +4698,16 @@
         <v>12</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" s="1">
+        <v>25</v>
+      </c>
+      <c r="M21" s="3">
         <v>7</v>
       </c>
       <c r="N21" s="19">
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -4850,19 +4717,19 @@
       <c r="D22" s="16">
         <v>3</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="3">
         <f t="shared" ref="E22:E25" si="1">F21</f>
         <v>53.16</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="3">
         <f t="shared" ref="F22:F25" si="2">E22+$E$14</f>
         <v>67.66</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="3">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E22,$B$3:$B$37,"&lt;"&amp;F22)</f>
         <v>13</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="3">
         <v>13</v>
       </c>
       <c r="I22" s="17">
@@ -4874,16 +4741,16 @@
         <v>25</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22" s="1">
+        <v>26</v>
+      </c>
+      <c r="M22" s="3">
         <v>13</v>
       </c>
       <c r="N22" s="19">
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -4893,19 +4760,19 @@
       <c r="D23" s="16">
         <v>4</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="3">
         <f t="shared" si="1"/>
         <v>67.66</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="3">
         <f t="shared" si="2"/>
         <v>82.16</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="3">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E23,$B$3:$B$37,"&lt;"&amp;F23)</f>
         <v>4</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="3">
         <v>4</v>
       </c>
       <c r="I23" s="17">
@@ -4917,16 +4784,16 @@
         <v>29</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" s="1">
+        <v>27</v>
+      </c>
+      <c r="M23" s="3">
         <v>4</v>
       </c>
       <c r="N23" s="19">
         <v>0.82857142857142863</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -4936,19 +4803,19 @@
       <c r="D24" s="16">
         <v>5</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="3">
         <f t="shared" si="1"/>
         <v>82.16</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="3">
         <f t="shared" si="2"/>
         <v>96.66</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="3">
         <f>COUNTIFS($B$3:$B$37,"&gt;="&amp;E24,$B$3:$B$37,"&lt;"&amp;F24)</f>
         <v>4</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="3">
         <v>4</v>
       </c>
       <c r="I24" s="17">
@@ -4960,16 +4827,16 @@
         <v>33</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="1">
+        <v>28</v>
+      </c>
+      <c r="M24" s="3">
         <v>4</v>
       </c>
       <c r="N24" s="19">
         <v>0.94285714285714284</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -5003,7 +4870,7 @@
         <v>35</v>
       </c>
       <c r="L25" s="20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M25" s="11">
         <v>2</v>
@@ -5012,7 +4879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -5021,7 +4888,7 @@
       </c>
       <c r="H26" s="24"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -5029,7 +4896,7 @@
         <v>65.31</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -5046,7 +4913,7 @@
       <c r="I28" s="26"/>
       <c r="J28" s="26"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -5055,7 +4922,7 @@
       </c>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -5066,17 +4933,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" s="5">
         <v>79.12</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="3">
         <f>AVERAGE(B3:B37)</f>
         <v>60</v>
       </c>
@@ -5084,14 +4951,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>30</v>
       </c>
       <c r="B32" s="5">
         <v>84.34</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G32" s="7">
@@ -5102,33 +4969,33 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" s="5">
         <v>86.89</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="3">
         <f>E79</f>
         <v>58.959999999999994</v>
       </c>
       <c r="I33" s="27"/>
     </row>
-    <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.4">
       <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" s="5">
         <v>91.74</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="3">
         <f>_xlfn.QUARTILE.INC($B$3:$B$37,1)</f>
         <v>47.584999999999994</v>
       </c>
@@ -5136,17 +5003,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.4">
       <c r="A35" s="5">
         <v>33</v>
       </c>
       <c r="B35" s="5">
         <v>96.01</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="3">
         <f>_xlfn.QUARTILE.INC($B$3:$B$37,2)</f>
         <v>56.8</v>
       </c>
@@ -5154,17 +5021,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.4">
       <c r="A36" s="5">
         <v>34</v>
       </c>
       <c r="B36" s="5">
         <v>106.84</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="3">
         <f>_xlfn.QUARTILE.INC($B$3:$B$37,3)</f>
         <v>70.314999999999998</v>
       </c>
@@ -5172,17 +5039,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>35</v>
       </c>
       <c r="B37" s="5">
         <v>111.16</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="3">
         <f>_xlfn.PERCENTILE.INC($B$3:$B$37,1/3)</f>
         <v>53.08</v>
       </c>
@@ -5190,19 +5057,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="28"/>
       <c r="B38" s="28"/>
       <c r="I38" s="27"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
         <v>45</v>
       </c>
       <c r="I39" s="27"/>
     </row>
-    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="s">
+    <row r="40" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="D40" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G40" s="29">
@@ -5213,8 +5080,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="1" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="3" t="s">
         <v>48</v>
       </c>
       <c r="G41" s="29">
@@ -5225,8 +5092,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="1" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D42" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G42" s="30">
@@ -5237,148 +5104,148 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D43" s="4"/>
       <c r="I43" s="31"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D44" s="4"/>
       <c r="I44" s="31"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
         <v>52</v>
       </c>
       <c r="I45" s="31"/>
     </row>
-    <row r="46" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D46" s="32"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
       <c r="I46" s="31"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D47" s="33" t="s">
         <v>53</v>
       </c>
       <c r="E47" s="33"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
       <c r="I47" s="31"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D49" s="1" t="s">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D49" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="3">
         <v>60</v>
       </c>
       <c r="I49" s="31"/>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D50" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="3">
         <v>3.620926618951553</v>
       </c>
       <c r="I50" s="31"/>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D51" s="1" t="s">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D51" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="3">
         <v>56.8</v>
       </c>
       <c r="I51" s="31"/>
     </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D52" s="1" t="s">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D52" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G52" s="1" t="e">
+      <c r="G52" s="3" t="e">
         <v>#N/A</v>
       </c>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D53" s="1" t="s">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D53" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G53" s="3">
         <v>21.421690766466529</v>
       </c>
       <c r="I53" s="31"/>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D54" s="1" t="s">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D54" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G54" s="3">
         <v>458.88883529411737</v>
       </c>
       <c r="I54" s="31"/>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="1" t="s">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D55" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G55" s="3">
         <v>0.14905801050987311</v>
       </c>
       <c r="I55" s="31"/>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D56" s="1" t="s">
+    <row r="56" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D56" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G56" s="1">
-        <v>0.60932074068833608</v>
+      <c r="G56" s="3">
+        <v>0.60932074068833597</v>
       </c>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="1" t="s">
+    <row r="57" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D57" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G57" s="1">
+      <c r="G57" s="3">
         <v>87</v>
       </c>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D58" s="1" t="s">
+    <row r="58" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D58" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G58" s="1">
+      <c r="G58" s="3">
         <v>24.16</v>
       </c>
       <c r="I58" s="31"/>
     </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
+    <row r="59" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D59" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G59" s="1">
+      <c r="G59" s="3">
         <v>111.16</v>
       </c>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D60" s="1" t="s">
+    <row r="60" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D60" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G60" s="1">
+      <c r="G60" s="3">
         <v>2100</v>
       </c>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D61" s="26" t="s">
         <v>66</v>
       </c>
@@ -5389,35 +5256,35 @@
       </c>
       <c r="I61" s="31"/>
     </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D62" s="4"/>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:9" x14ac:dyDescent="0.3">
       <c r="I63" s="31"/>
     </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D64" s="34" t="s">
         <v>57</v>
       </c>
       <c r="I64" s="31"/>
     </row>
-    <row r="65" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D65" s="1" t="s">
+    <row r="65" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D65" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D66" s="1" t="s">
+    <row r="66" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D66" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D68" s="1" t="s">
+    <row r="68" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D68" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D74" s="35" t="s">
         <v>70</v>
       </c>
@@ -5425,11 +5292,11 @@
         <f>E22</f>
         <v>53.16</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="G74" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D75" s="35" t="s">
         <v>72</v>
       </c>
@@ -5437,11 +5304,11 @@
         <f>F22-E22</f>
         <v>14.5</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="G75" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="4:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:10" ht="18" x14ac:dyDescent="0.4">
       <c r="D76" s="35" t="s">
         <v>74</v>
       </c>
@@ -5449,11 +5316,11 @@
         <f>G22</f>
         <v>13</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="G76" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="4:10" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:10" ht="18" x14ac:dyDescent="0.4">
       <c r="D77" s="35" t="s">
         <v>76</v>
       </c>
@@ -5461,11 +5328,11 @@
         <f>G21</f>
         <v>7</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="G77" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="4:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="4:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
       <c r="D78" s="36" t="s">
         <v>78</v>
       </c>
@@ -5481,7 +5348,7 @@
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
     </row>
-    <row r="79" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D79" s="37" t="s">
         <v>80</v>
       </c>
@@ -5495,21 +5362,21 @@
       </c>
       <c r="H79" s="39"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D86" s="4"/>
     </row>
-    <row r="100" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:19" x14ac:dyDescent="0.3">
       <c r="Q100" s="29"/>
       <c r="R100" s="29"/>
       <c r="S100" s="29"/>
     </row>
-    <row r="105" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E105" s="19"/>
     </row>
-    <row r="106" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E106" s="19"/>
     </row>
-    <row r="107" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:19" x14ac:dyDescent="0.3">
       <c r="E107" s="19"/>
     </row>
   </sheetData>

</xml_diff>